<commit_message>
Update Milestone 1 folder for submission
</commit_message>
<xml_diff>
--- a/Milestone 1/Product backlog.xlsx
+++ b/Milestone 1/Product backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\RMIT\5SEPT\12_Bin_Chickens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\RMIT\5SEPT\12_Bin_Chickens\ND_Telemedicine_App\Milestone 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67F7AAE-BF06-466B-9965-12F73891287F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3FD71A-0813-4F25-9EE3-2DF7DCF11C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="3855" windowWidth="19230" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9975" yWindow="3840" windowWidth="19230" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="141">
   <si>
     <t>ID</t>
   </si>
@@ -640,6 +640,18 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>Luke, Ash</t>
+  </si>
+  <si>
+    <t>Joseph, Abdul</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amy </t>
   </si>
 </sst>
 </file>
@@ -1338,8 +1350,8 @@
   </sheetPr>
   <dimension ref="A2:K91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1434,7 +1446,9 @@
       <c r="E5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="13" t="s">
+        <v>137</v>
+      </c>
       <c r="G5" s="15" t="s">
         <v>41</v>
       </c>
@@ -1461,7 +1475,9 @@
       <c r="E6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G6" s="28"/>
       <c r="H6" s="37"/>
       <c r="I6" s="28"/>
@@ -1480,7 +1496,9 @@
       <c r="E7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G7" s="28"/>
       <c r="H7" s="37"/>
       <c r="I7" s="28"/>
@@ -1499,7 +1517,9 @@
       <c r="E8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G8" s="28"/>
       <c r="H8" s="37"/>
       <c r="I8" s="28"/>
@@ -1518,7 +1538,9 @@
       <c r="E9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G9" s="28"/>
       <c r="H9" s="37"/>
       <c r="I9" s="28"/>
@@ -1537,7 +1559,9 @@
       <c r="E10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G10" s="28"/>
       <c r="H10" s="37"/>
       <c r="I10" s="28"/>
@@ -1558,7 +1582,9 @@
       <c r="E11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G11" s="31" t="s">
         <v>41</v>
       </c>
@@ -1585,7 +1611,9 @@
       <c r="E12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G12" s="28"/>
       <c r="H12" s="37"/>
       <c r="I12" s="28"/>
@@ -1604,7 +1632,9 @@
       <c r="E13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G13" s="28"/>
       <c r="H13" s="37"/>
       <c r="I13" s="28"/>
@@ -1623,7 +1653,9 @@
       <c r="E14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G14" s="28"/>
       <c r="H14" s="37"/>
       <c r="I14" s="28"/>
@@ -1642,7 +1674,9 @@
       <c r="E15" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G15" s="28"/>
       <c r="H15" s="37"/>
       <c r="I15" s="28"/>
@@ -1661,7 +1695,9 @@
       <c r="E16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="G16" s="28"/>
       <c r="H16" s="37"/>
       <c r="I16" s="28"/>
@@ -1682,7 +1718,9 @@
       <c r="E17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G17" s="28" t="s">
         <v>41</v>
       </c>
@@ -1709,7 +1747,9 @@
       <c r="E18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G18" s="28"/>
       <c r="H18" s="37"/>
       <c r="I18" s="28"/>
@@ -1728,7 +1768,9 @@
       <c r="E19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>
       <c r="I19" s="28"/>
@@ -1747,7 +1789,9 @@
       <c r="E20" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="14"/>
+      <c r="F20" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G20" s="28"/>
       <c r="H20" s="37"/>
       <c r="I20" s="28"/>
@@ -1766,7 +1810,9 @@
       <c r="E21" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G21" s="28"/>
       <c r="H21" s="37"/>
       <c r="I21" s="28"/>
@@ -1785,7 +1831,9 @@
       <c r="E22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G22" s="28"/>
       <c r="H22" s="37"/>
       <c r="I22" s="28"/>
@@ -1806,7 +1854,9 @@
       <c r="E23" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G23" s="28" t="s">
         <v>41</v>
       </c>
@@ -1833,7 +1883,9 @@
       <c r="E24" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G24" s="28"/>
       <c r="H24" s="37"/>
       <c r="I24" s="28"/>
@@ -1852,7 +1904,9 @@
       <c r="E25" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="14"/>
+      <c r="F25" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G25" s="28"/>
       <c r="H25" s="37"/>
       <c r="I25" s="28"/>
@@ -1871,7 +1925,9 @@
       <c r="E26" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G26" s="28"/>
       <c r="H26" s="37"/>
       <c r="I26" s="28"/>
@@ -1892,7 +1948,9 @@
       <c r="E27" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G27" s="28" t="s">
         <v>41</v>
       </c>
@@ -1919,7 +1977,9 @@
       <c r="E28" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G28" s="28"/>
       <c r="H28" s="37"/>
       <c r="I28" s="28"/>
@@ -1938,7 +1998,9 @@
       <c r="E29" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="14"/>
+      <c r="F29" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G29" s="32"/>
       <c r="H29" s="38"/>
       <c r="I29" s="32"/>
@@ -1957,7 +2019,9 @@
       <c r="E30" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="14"/>
+      <c r="F30" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G30" s="28"/>
       <c r="H30" s="37"/>
       <c r="I30" s="28"/>
@@ -1976,14 +2040,16 @@
       <c r="E31" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F31" s="14"/>
+      <c r="F31" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G31" s="28"/>
       <c r="H31" s="37"/>
       <c r="I31" s="28"/>
       <c r="J31" s="22"/>
       <c r="K31" s="22"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="21">
         <v>5</v>
@@ -1995,7 +2061,9 @@
       <c r="E32" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="F32" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G32" s="28"/>
       <c r="H32" s="37"/>
       <c r="I32" s="28"/>
@@ -2016,7 +2084,9 @@
       <c r="E33" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="14"/>
+      <c r="F33" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G33" s="28" t="s">
         <v>41</v>
       </c>
@@ -2043,7 +2113,9 @@
       <c r="E34" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G34" s="28"/>
       <c r="H34" s="37"/>
       <c r="I34" s="28"/>
@@ -2062,7 +2134,9 @@
       <c r="E35" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G35" s="28"/>
       <c r="H35" s="37"/>
       <c r="I35" s="28"/>
@@ -2081,7 +2155,9 @@
       <c r="E36" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="14"/>
+      <c r="F36" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G36" s="28"/>
       <c r="H36" s="37"/>
       <c r="I36" s="28"/>
@@ -2100,7 +2176,9 @@
       <c r="E37" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F37" s="14"/>
+      <c r="F37" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G37" s="28"/>
       <c r="H37" s="37"/>
       <c r="I37" s="28"/>
@@ -2119,7 +2197,9 @@
       <c r="E38" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="14"/>
+      <c r="F38" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="G38" s="28"/>
       <c r="H38" s="37"/>
       <c r="I38" s="28"/>
@@ -2138,7 +2218,9 @@
       <c r="E39" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="14"/>
+      <c r="F39" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="G39" s="28"/>
       <c r="H39" s="37"/>
       <c r="I39" s="28"/>

</xml_diff>